<commit_message>
Adding in Tranche 2 spreadheets: fixing ZM07
</commit_message>
<xml_diff>
--- a/zm_expandabilityfactors.xlsx
+++ b/zm_expandabilityfactors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -1294,7 +1294,7 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
       <selection pane="topRight" activeCell="G95" sqref="G95"/>

</xml_diff>

<commit_message>
Added in Tranche 2 spreadheet: fixing ZM12
</commit_message>
<xml_diff>
--- a/zm_expandabilityfactors.xlsx
+++ b/zm_expandabilityfactors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -1294,7 +1294,7 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
       <selection pane="topRight" activeCell="G95" sqref="G95"/>

</xml_diff>

<commit_message>
Added in Tranche 2 spreadsheet: ZM13, fixing ZM12
</commit_message>
<xml_diff>
--- a/zm_expandabilityfactors.xlsx
+++ b/zm_expandabilityfactors.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="115">
   <si>
     <t>WEALTH GROUP</t>
   </si>
@@ -336,9 +336,6 @@
     <t>Additional Price (per kg)</t>
   </si>
   <si>
-    <t>fpl</t>
-  </si>
-  <si>
     <t>des</t>
   </si>
   <si>
@@ -436,6 +433,12 @@
   </si>
   <si>
     <t>loquats</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>mns</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +516,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,7 +713,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -793,6 +808,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="72">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1294,10 +1311,10 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="G95" sqref="G95"/>
+      <selection pane="topRight" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1320,10 +1337,10 @@
         <v>2100</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="51" t="s">
         <v>91</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>92</v>
       </c>
       <c r="F1" s="50">
         <f>IF(UPPER(D1)="KJ",4.1868,IF(OR(UPPER(D1)="KCAL",AND(CODE(LEFT(D1))=67,UPPER(MID(D1,2,LEN(D1)-1))="AL")),1,IF(AND(CODE(LEFT(D1))=99,UPPER(MID(D1,2,LEN(D1)-1))="AL"),1000,0)))</f>
@@ -1882,7 +1899,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="53" t="s">
         <v>68</v>
@@ -1896,12 +1913,12 @@
       <c r="H42" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="I42" s="18" t="s">
+      <c r="I42" s="46" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="13">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="56" t="s">
         <v>74</v>
       </c>
       <c r="B43" s="30" t="s">
@@ -1924,8 +1941,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="13">
-      <c r="A44" s="43" t="s">
-        <v>93</v>
+      <c r="A44" s="57" t="s">
+        <v>92</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>77</v>
@@ -1943,12 +1960,12 @@
         <v>1</v>
       </c>
       <c r="I44" s="18" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="13">
-      <c r="A45" s="43" t="s">
-        <v>94</v>
+      <c r="A45" s="57" t="s">
+        <v>93</v>
       </c>
       <c r="B45" s="30" t="s">
         <v>77</v>
@@ -1966,12 +1983,12 @@
         <v>1</v>
       </c>
       <c r="I45" s="18" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13">
-      <c r="A46" s="43" t="s">
-        <v>95</v>
+      <c r="A46" s="56" t="s">
+        <v>94</v>
       </c>
       <c r="B46" s="30" t="s">
         <v>77</v>
@@ -1993,8 +2010,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="13">
-      <c r="A47" s="43" t="s">
-        <v>96</v>
+      <c r="A47" s="56" t="s">
+        <v>95</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>77</v>
@@ -2017,7 +2034,7 @@
     </row>
     <row r="48" spans="1:9" ht="13">
       <c r="A48" s="43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>77</v>
@@ -2035,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="13">
@@ -2058,12 +2075,12 @@
         <v>1</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="13">
       <c r="A50" s="44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" s="39" t="s">
         <v>77</v>
@@ -2086,7 +2103,7 @@
     </row>
     <row r="51" spans="1:9" ht="13">
       <c r="A51" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" s="30" t="s">
         <v>77</v>
@@ -2132,7 +2149,7 @@
     </row>
     <row r="53" spans="1:9" ht="13">
       <c r="A53" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B53" s="30" t="s">
         <v>77</v>
@@ -2155,7 +2172,7 @@
     </row>
     <row r="54" spans="1:9" ht="13">
       <c r="A54" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B54" s="30" t="s">
         <v>77</v>
@@ -2173,12 +2190,12 @@
         <v>1</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13">
       <c r="A55" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="30" t="s">
         <v>77</v>
@@ -2201,7 +2218,7 @@
     </row>
     <row r="56" spans="1:9" ht="13">
       <c r="A56" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" s="30" t="s">
         <v>77</v>
@@ -2242,12 +2259,12 @@
         <v>1</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13">
       <c r="A58" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B58" s="30" t="s">
         <v>77</v>
@@ -2265,12 +2282,12 @@
         <v>1</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="13">
       <c r="A59" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B59" s="30" t="s">
         <v>77</v>
@@ -2293,7 +2310,7 @@
     </row>
     <row r="60" spans="1:9" ht="13">
       <c r="A60" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B60" s="30" t="s">
         <v>77</v>
@@ -2316,7 +2333,7 @@
     </row>
     <row r="61" spans="1:9" ht="13">
       <c r="A61" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B61" s="30" t="s">
         <v>77</v>
@@ -2339,7 +2356,7 @@
     </row>
     <row r="62" spans="1:9" ht="13">
       <c r="A62" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B62" s="30" t="s">
         <v>77</v>
@@ -2362,7 +2379,7 @@
     </row>
     <row r="63" spans="1:9" ht="13">
       <c r="A63" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B63" s="30" t="s">
         <v>77</v>
@@ -2385,7 +2402,7 @@
     </row>
     <row r="64" spans="1:9" ht="13">
       <c r="A64" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="30" t="s">
         <v>77</v>
@@ -2403,12 +2420,12 @@
         <v>1</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="13">
       <c r="A65" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B65" s="30" t="s">
         <v>77</v>
@@ -2426,12 +2443,12 @@
         <v>1</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="13">
       <c r="A66" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B66" s="30" t="s">
         <v>77</v>
@@ -2449,12 +2466,12 @@
         <v>1</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="13">
       <c r="A67" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B67" s="30" t="s">
         <v>77</v>
@@ -2472,12 +2489,12 @@
         <v>1</v>
       </c>
       <c r="I67" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="13">
       <c r="A68" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B68" s="30" t="s">
         <v>77</v>
@@ -2495,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="I68" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="13">
@@ -2518,7 +2535,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="13">
@@ -2526,7 +2543,7 @@
         <v>32</v>
       </c>
       <c r="B70" s="47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C70" s="53" t="s">
         <v>68</v>
@@ -2564,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="I71" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="13">
@@ -2590,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="I72" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="13">
@@ -2620,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="13">
@@ -2646,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="13">
@@ -2672,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13">
@@ -2698,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13">
@@ -2724,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13">
@@ -2751,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="I78" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13">
@@ -2779,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13">
@@ -2805,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13">
@@ -2831,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="13">
@@ -2851,12 +2868,12 @@
         <v>0</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="13">
       <c r="A83" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83" s="33"/>
       <c r="C83" s="53" t="s">
@@ -2874,7 +2891,7 @@
     </row>
     <row r="84" spans="1:9" ht="13">
       <c r="A84" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" s="30" t="s">
         <v>77</v>
@@ -2892,12 +2909,12 @@
         <v>1</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="13">
       <c r="A85" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B85" s="30" t="s">
         <v>77</v>
@@ -2915,12 +2932,12 @@
         <v>1</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="13">
       <c r="A86" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" s="33"/>
       <c r="C86" s="53" t="s">
@@ -2959,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="13">
@@ -2979,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="13">
@@ -3017,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="13">
@@ -3043,7 +3060,7 @@
         <v>0</v>
       </c>
       <c r="I91" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="13">
@@ -3090,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="13">
@@ -3110,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="I94" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="13">
@@ -3154,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="I96" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="13">
@@ -3180,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="I97" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="13">
@@ -3206,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="I98" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="13">
@@ -3232,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="I99" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="13">
@@ -3258,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="I100" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="13">
@@ -3284,7 +3301,7 @@
         <v>0</v>
       </c>
       <c r="I101" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="13">
@@ -3310,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="I102" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="13">
@@ -3336,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="I103" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="13">
@@ -3362,7 +3379,7 @@
         <v>0</v>
       </c>
       <c r="I104" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="13">
@@ -3388,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="I105" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:9">

</xml_diff>

<commit_message>
Corrections to ZM03, ZM07, ZM12, exp_factors
</commit_message>
<xml_diff>
--- a/zm_expandabilityfactors.xlsx
+++ b/zm_expandabilityfactors.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="112">
   <si>
     <t>WEALTH GROUP</t>
   </si>
@@ -339,16 +339,7 @@
     <t>des</t>
   </si>
   <si>
-    <t>lbpl</t>
-  </si>
-  <si>
     <t>beef</t>
-  </si>
-  <si>
-    <t>dis</t>
-  </si>
-  <si>
-    <t>ubpl</t>
   </si>
   <si>
     <t>Poverty Lines</t>
@@ -799,6 +790,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -808,8 +801,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="72">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1311,10 +1302,10 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="I48" sqref="I48"/>
+      <selection pane="topRight" activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1337,10 +1328,10 @@
         <v>2100</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="50">
         <f>IF(UPPER(D1)="KJ",4.1868,IF(OR(UPPER(D1)="KCAL",AND(CODE(LEFT(D1))=67,UPPER(MID(D1,2,LEN(D1)-1))="AL")),1,IF(AND(CODE(LEFT(D1))=99,UPPER(MID(D1,2,LEN(D1)-1))="AL"),1000,0)))</f>
@@ -1899,14 +1890,14 @@
         <v>28</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="55"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="57"/>
       <c r="G42" s="46" t="s">
         <v>78</v>
       </c>
@@ -1918,7 +1909,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="13">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="53" t="s">
         <v>74</v>
       </c>
       <c r="B43" s="30" t="s">
@@ -1941,8 +1932,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="13">
-      <c r="A44" s="57" t="s">
-        <v>92</v>
+      <c r="A44" s="54" t="s">
+        <v>89</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>77</v>
@@ -1960,12 +1951,12 @@
         <v>1</v>
       </c>
       <c r="I44" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="13">
-      <c r="A45" s="57" t="s">
-        <v>93</v>
+      <c r="A45" s="54" t="s">
+        <v>90</v>
       </c>
       <c r="B45" s="30" t="s">
         <v>77</v>
@@ -1983,12 +1974,12 @@
         <v>1</v>
       </c>
       <c r="I45" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13">
-      <c r="A46" s="56" t="s">
-        <v>94</v>
+      <c r="A46" s="53" t="s">
+        <v>91</v>
       </c>
       <c r="B46" s="30" t="s">
         <v>77</v>
@@ -2010,8 +2001,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="13">
-      <c r="A47" s="56" t="s">
-        <v>95</v>
+      <c r="A47" s="53" t="s">
+        <v>92</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>77</v>
@@ -2034,7 +2025,7 @@
     </row>
     <row r="48" spans="1:9" ht="13">
       <c r="A48" s="43" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>77</v>
@@ -2052,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="13">
@@ -2075,12 +2066,12 @@
         <v>1</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="13">
       <c r="A50" s="44" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B50" s="39" t="s">
         <v>77</v>
@@ -2103,7 +2094,7 @@
     </row>
     <row r="51" spans="1:9" ht="13">
       <c r="A51" s="43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B51" s="30" t="s">
         <v>77</v>
@@ -2149,7 +2140,7 @@
     </row>
     <row r="53" spans="1:9" ht="13">
       <c r="A53" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" s="30" t="s">
         <v>77</v>
@@ -2172,7 +2163,7 @@
     </row>
     <row r="54" spans="1:9" ht="13">
       <c r="A54" s="43" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B54" s="30" t="s">
         <v>77</v>
@@ -2190,12 +2181,12 @@
         <v>1</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13">
       <c r="A55" s="43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B55" s="30" t="s">
         <v>77</v>
@@ -2218,7 +2209,7 @@
     </row>
     <row r="56" spans="1:9" ht="13">
       <c r="A56" s="43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B56" s="30" t="s">
         <v>77</v>
@@ -2259,12 +2250,12 @@
         <v>1</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13">
       <c r="A58" s="43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B58" s="30" t="s">
         <v>77</v>
@@ -2282,12 +2273,12 @@
         <v>1</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="13">
       <c r="A59" s="43" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B59" s="30" t="s">
         <v>77</v>
@@ -2310,7 +2301,7 @@
     </row>
     <row r="60" spans="1:9" ht="13">
       <c r="A60" s="43" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B60" s="30" t="s">
         <v>77</v>
@@ -2333,7 +2324,7 @@
     </row>
     <row r="61" spans="1:9" ht="13">
       <c r="A61" s="43" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B61" s="30" t="s">
         <v>77</v>
@@ -2356,7 +2347,7 @@
     </row>
     <row r="62" spans="1:9" ht="13">
       <c r="A62" s="43" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B62" s="30" t="s">
         <v>77</v>
@@ -2379,7 +2370,7 @@
     </row>
     <row r="63" spans="1:9" ht="13">
       <c r="A63" s="43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B63" s="30" t="s">
         <v>77</v>
@@ -2402,7 +2393,7 @@
     </row>
     <row r="64" spans="1:9" ht="13">
       <c r="A64" s="43" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B64" s="30" t="s">
         <v>77</v>
@@ -2420,12 +2411,12 @@
         <v>1</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="13">
       <c r="A65" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B65" s="30" t="s">
         <v>77</v>
@@ -2443,12 +2434,12 @@
         <v>1</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="13">
       <c r="A66" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B66" s="30" t="s">
         <v>77</v>
@@ -2471,7 +2462,7 @@
     </row>
     <row r="67" spans="1:9" ht="13">
       <c r="A67" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B67" s="30" t="s">
         <v>77</v>
@@ -2494,7 +2485,7 @@
     </row>
     <row r="68" spans="1:9" ht="13">
       <c r="A68" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B68" s="30" t="s">
         <v>77</v>
@@ -2535,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="13">
@@ -2543,14 +2534,14 @@
         <v>32</v>
       </c>
       <c r="B70" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="C70" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="55"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="57"/>
       <c r="G70" s="46" t="s">
         <v>69</v>
       </c>
@@ -2581,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="I71" s="18" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="13">
@@ -2607,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="I72" s="18" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="13">
@@ -2637,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="18" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="13">
@@ -2663,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="13">
@@ -2689,7 +2680,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="18" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13">
@@ -2715,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13">
@@ -2768,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="I78" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13">
@@ -2796,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13">
@@ -2822,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13">
@@ -2848,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="13">
@@ -2868,20 +2859,20 @@
         <v>0</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="13">
       <c r="A83" s="32" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B83" s="33"/>
-      <c r="C83" s="53" t="s">
+      <c r="C83" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D83" s="54"/>
-      <c r="E83" s="54"/>
-      <c r="F83" s="55"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="56"/>
+      <c r="F83" s="57"/>
       <c r="G83" s="46" t="s">
         <v>69</v>
       </c>
@@ -2891,7 +2882,7 @@
     </row>
     <row r="84" spans="1:9" ht="13">
       <c r="A84" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B84" s="30" t="s">
         <v>77</v>
@@ -2909,12 +2900,12 @@
         <v>1</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="13">
       <c r="A85" s="34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B85" s="30" t="s">
         <v>77</v>
@@ -2932,20 +2923,20 @@
         <v>1</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="13">
       <c r="A86" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B86" s="33"/>
-      <c r="C86" s="53" t="s">
+      <c r="C86" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D86" s="54"/>
-      <c r="E86" s="54"/>
-      <c r="F86" s="55"/>
+      <c r="D86" s="56"/>
+      <c r="E86" s="56"/>
+      <c r="F86" s="57"/>
       <c r="G86" s="46" t="s">
         <v>69</v>
       </c>
@@ -2996,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="13">
@@ -3004,12 +2995,12 @@
         <v>40</v>
       </c>
       <c r="B89" s="33"/>
-      <c r="C89" s="53" t="s">
+      <c r="C89" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D89" s="54"/>
-      <c r="E89" s="54"/>
-      <c r="F89" s="55"/>
+      <c r="D89" s="56"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="57"/>
       <c r="G89" s="46" t="s">
         <v>69</v>
       </c>
@@ -3034,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="18" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="13">
@@ -3068,12 +3059,12 @@
         <v>43</v>
       </c>
       <c r="B92" s="33"/>
-      <c r="C92" s="53" t="s">
+      <c r="C92" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D92" s="54"/>
-      <c r="E92" s="54"/>
-      <c r="F92" s="55"/>
+      <c r="D92" s="56"/>
+      <c r="E92" s="56"/>
+      <c r="F92" s="57"/>
       <c r="G92" s="46" t="s">
         <v>69</v>
       </c>
@@ -3107,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="13">
@@ -3127,7 +3118,7 @@
         <v>0</v>
       </c>
       <c r="I94" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="13">
@@ -3135,12 +3126,12 @@
         <v>46</v>
       </c>
       <c r="B95" s="33"/>
-      <c r="C95" s="53" t="s">
+      <c r="C95" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D95" s="54"/>
-      <c r="E95" s="54"/>
-      <c r="F95" s="55"/>
+      <c r="D95" s="56"/>
+      <c r="E95" s="56"/>
+      <c r="F95" s="57"/>
       <c r="G95" s="46" t="s">
         <v>69</v>
       </c>

</xml_diff>